<commit_message>
Finished ETL for Baumgartner_C-N.
Signed-off-by: Daniel Wigh <dswigh@gmail.com>
</commit_message>
<xml_diff>
--- a/data/baumgartner_C-N/op9b00236_si_002.xlsx
+++ b/data/baumgartner_C-N/op9b00236_si_002.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10711"/>
   <workbookPr filterPrivacy="1"/>
   <xr:revisionPtr revIDLastSave="1" documentId="11_4670260951FF86F7124ECD50E489A0D024BC05DD" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BDC9E849-247B-E94B-A628-0ACB8CE178D5}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" tabRatio="961" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15960" tabRatio="961" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Optimization overview" sheetId="2" r:id="rId1"/>
@@ -4752,8 +4752,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O91"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7811,7 +7811,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:X375"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>

<commit_message>
Add back in .pb files
</commit_message>
<xml_diff>
--- a/data/baumgartner_C-N/op9b00236_si_002.xlsx
+++ b/data/baumgartner_C-N/op9b00236_si_002.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10912"/>
   <workbookPr filterPrivacy="1"/>
   <xr:revisionPtr revIDLastSave="1" documentId="11_4670260951FF86F7124ECD50E489A0D024BC05DD" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BDC9E849-247B-E94B-A628-0ACB8CE178D5}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15960" tabRatio="961" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15880" tabRatio="961" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Optimization overview" sheetId="2" r:id="rId1"/>
@@ -40,6 +40,13 @@
     </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>

</xml_diff>